<commit_message>
Adaption of Excels (remove whitespaces in column GapType!)
</commit_message>
<xml_diff>
--- a/inst/shiny-apps/vsim/data/outputs/Testcase_aeltere_Arbeitnehmer_Arbeit.xlsx
+++ b/inst/shiny-apps/vsim/data/outputs/Testcase_aeltere_Arbeitnehmer_Arbeit.xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SLC\Desktop\IMS\packages\vsim\inst\shiny-apps\vsim\data\outputs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438FBC22-1C0B-4FB7-BF23-AFA97ECDF35C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="QAGlist_Teil1" r:id="rId3" sheetId="1"/>
+    <sheet name="QAGlist_Teil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -278,17 +286,16 @@
     <t>Privat</t>
   </si>
   <si>
-    <t>Arbeit, Privat</t>
+    <t>Arbeit,Privat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -300,7 +307,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -318,18 +325,328 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -370,7 +687,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -411,7 +728,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -452,7 +769,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -493,7 +810,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -534,7 +851,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -575,7 +892,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -616,7 +933,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -657,7 +974,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -698,7 +1015,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -739,7 +1056,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -780,7 +1097,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -821,7 +1138,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -862,7 +1179,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -903,7 +1220,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -944,7 +1261,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -985,7 +1302,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1026,7 +1343,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1067,7 +1384,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1108,7 +1425,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1149,7 +1466,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1190,7 +1507,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1231,7 +1548,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1272,7 +1589,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1313,7 +1630,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1354,7 +1671,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1395,7 +1712,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1436,7 +1753,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1477,7 +1794,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -1518,7 +1835,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -1560,6 +1877,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>